<commit_message>
Added column mapping listing api
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abd2\Documents\Edith\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokkumar.ext\Documents\projects\node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60715EC6-9B9A-4798-B159-55912676EF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF592DE8-0803-4D38-A012-428B5DFD0282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DE76C75-D052-46FA-8D2E-A392091CC3BB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6DE76C75-D052-46FA-8D2E-A392091CC3BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Source</t>
   </si>
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,15 +462,15 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -486,7 +486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -494,7 +494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -502,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -510,15 +510,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -526,7 +523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -534,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -542,15 +539,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -558,63 +552,42 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -622,10 +595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>20</v>
       </c>

</xml_diff>